<commit_message>
Update August 2025 retrospective data
- Updated August 2025 Release Retrospective (Responses).xlsx with latest data
- Ensures data consistency with recent fixes to director trends analysis
- Maintains data integrity across all analysis components
</commit_message>
<xml_diff>
--- a/Retrospectives/August 2025 Release Retrospective (Responses).xlsx
+++ b/Retrospectives/August 2025 Release Retrospective (Responses).xlsx
@@ -5,22 +5,24 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajendran/Documents/Retrospective Analysis/Retrospectives/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajendran/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E410484C-C78B-384B-94E9-AF4E71A4E411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF046A68-53D1-EB49-870F-4A3B1EAB29A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Pivot Table 1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5714" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6279" uniqueCount="1018">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2839,6 +2841,304 @@
   </si>
   <si>
     <t>claide-4-sonet, opus &amp; Auto</t>
+  </si>
+  <si>
+    <t>Inceris</t>
+  </si>
+  <si>
+    <t>Building Dashboards</t>
+  </si>
+  <si>
+    <t>Building Dashboards on Engineering productivity</t>
+  </si>
+  <si>
+    <t>Exploring / understanding existing codebase, Writing code for new features, Review PRs, Debugging and Fixing Bugs, Creating test cases or test scripts, Creating Workflows</t>
+  </si>
+  <si>
+    <t>I used Cursor for creating a Dashboard application for Cursor Metrics Analysis.
+I thought this is the right way to start with.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ya, I still use chatGPT, beyond the AI IDE,
+Chatgpt can have access of analysing multiple type file formats like pdf,word docs,videos and all
+and it has Multi-Project Knowledge which is not available in Cursor IDE
+</t>
+  </si>
+  <si>
+    <t>It will be better if Cursor has Multi-Project Knowledge which mean the data should have sync for different chats too.</t>
+  </si>
+  <si>
+    <t>Yes,We can have more on Slack</t>
+  </si>
+  <si>
+    <t>Ganges</t>
+  </si>
+  <si>
+    <t>action item to plan the release such that bandwidth is available to fix any last-minute bugs. Plan such that the code and testing is done atleast 2 days prior to the deadline</t>
+  </si>
+  <si>
+    <t>While doing the analysis for a spike, I provided cursor the context and the requirement sheet, it was able to write the code and generate documentation</t>
+  </si>
+  <si>
+    <t>No, not as of now</t>
+  </si>
+  <si>
+    <t>Better than Copilot, but needs improvement in integration with vscode.</t>
+  </si>
+  <si>
+    <t>Claude 4 sonnet</t>
+  </si>
+  <si>
+    <t>in sprint automation</t>
+  </si>
+  <si>
+    <t>Dev Prototype, Exploring / understanding existing codebase, Debugging and Fixing Bugs, Creating test cases or test scripts</t>
+  </si>
+  <si>
+    <t>I am QA but i fixed couple of bugs using cursor</t>
+  </si>
+  <si>
+    <t>Yes, code understanding and writing has been very accurate when i use cursor</t>
+  </si>
+  <si>
+    <t>Max mode for complex problems with claude sonnet  model</t>
+  </si>
+  <si>
+    <t>Yes getting all the support</t>
+  </si>
+  <si>
+    <t>Exploring / understanding existing codebase, Review PRs, Debugging and Fixing Bugs, Understanding estimates for bug fixes and new feature development</t>
+  </si>
+  <si>
+    <t>Was able to understand code changes require to separate out unit test cases which require third party connections and should go under integration suites.This also let me understand new set of technical debts and high level efforts required to plan them.</t>
+  </si>
+  <si>
+    <t>Yes. GPT helped me to explore designs and technology other then what we have in our code base such as which technology would benefit in which use case vs what we have and explore pros and cons of each to balance out approach and find technical debts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I use both GPT and Cursor. </t>
+  </si>
+  <si>
+    <t>Getting full support</t>
+  </si>
+  <si>
+    <t>proper planning based on bandwidth..we were able achieve with planning , 100% completed</t>
+  </si>
+  <si>
+    <t>"working on customer reported issue."
+We found that we have support on BE but not on UI on http pagination.
+Again we need confirm where we have the feasibility for all paging method or any specific.
+Able to check the feasibility on back end using cursor.
+Reference link: https://celigo-internal.slack.com/archives/CTK3RBK1D/p1752677177376509?thread_ts=1752640818.116669&amp;cid=CTK3RBK1D"</t>
+  </si>
+  <si>
+    <t>Problem Solving Outside Code, Documentation, Communication &amp; Reporting
+Summarizing tickets or logs into readable descriptions
+Writing bug reports, user stories, or Jira tasks
+Rewriting technical updates into polished, clear communication for various audiences (QA, PMs, leadership)</t>
+  </si>
+  <si>
+    <t>especially for prototyping, refactoring, or debugging. But it doesn’t eliminate the need for out-of-IDE thinking, which is where ChatGPT (browser or API) still shines.</t>
+  </si>
+  <si>
+    <t>Auto mode since it consumes less number of hits as per prompt</t>
+  </si>
+  <si>
+    <t>Better dependencies tracking - release alignment, status, risk and deviations must transparently call outs during the connects</t>
+  </si>
+  <si>
+    <t>Exploring / understanding existing codebase, Debugging and Fixing Bugs, Creating test cases or test scripts</t>
+  </si>
+  <si>
+    <t>For a given PR - Identifying the impacted areas and missing test cases from existing test coverage by scanning through the automation repo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, esp for test designs  and any other strategic initiatives recommendations and documentation part ChatGPT is helpful </t>
+  </si>
+  <si>
+    <t>MCP - Git Integration &amp; JIRA Integration are helpful</t>
+  </si>
+  <si>
+    <t>auto &amp; claude-3.5-sonnet</t>
+  </si>
+  <si>
+    <t>Exposing Agents/integrate with Jenkins, so that it has more visibility and others can use.</t>
+  </si>
+  <si>
+    <t>Design Reviews and Canary Planning</t>
+  </si>
+  <si>
+    <t>Dev Prototype, Exploring / understanding existing codebase, using chatgpt, gemni for design and exploration of new technologies eg: MCP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understanding existing code base and making changes for refactoring </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes.  I use for lot of research.   </t>
+  </si>
+  <si>
+    <t>At an Architect level, who don't involve in coding daily, cursor gives me great leaverage in understanding existing code and trying new things</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto &amp; Max. Sometimes switch the model myself. </t>
+  </si>
+  <si>
+    <t>Technical Design</t>
+  </si>
+  <si>
+    <t>Developing a POC to compare Schema Inferencing using Spark behind custom service vs Argo Workflow</t>
+  </si>
+  <si>
+    <t>Yes, At times the quality of output is superior with CgatGPT &amp; Codex</t>
+  </si>
+  <si>
+    <t>It is a bit more stable compared to couple of months ago</t>
+  </si>
+  <si>
+    <t>Improve in Jira tracker updates</t>
+  </si>
+  <si>
+    <t>While doing the integration deprecation task, It helps me in compare and find the missing api's in api-gateway and integrator. If we do this manually then it will take lot of time</t>
+  </si>
+  <si>
+    <t>It helps is designing and exploring new research related tasks</t>
+  </si>
+  <si>
+    <t>It's really good and increased a productivity</t>
+  </si>
+  <si>
+    <t>Helped in writing the tech design, reviewing it and identifying the edge cases.</t>
+  </si>
+  <si>
+    <t>It is very helpful</t>
+  </si>
+  <si>
+    <t>I was working on a PoC to handle some workload. Cursor was able to bring up 60% of code which was further customised based on the requirement.
+Although cursor was able to produce code and reiterate based on requirements, we have to verify the code being updated as 50% of time it will try to change code unnecessarily.</t>
+  </si>
+  <si>
+    <t>Few scenarios, but most of tasks can be completed by Cursor only</t>
+  </si>
+  <si>
+    <t>Increases speed of PoC or development.</t>
+  </si>
+  <si>
+    <t>Lunch n Learn</t>
+  </si>
+  <si>
+    <t>Better planning of dependencies and feature branch merges</t>
+  </si>
+  <si>
+    <t>Exploring understanding and fixing a bug in a service which i have never worked on</t>
+  </si>
+  <si>
+    <t>Yes Chatgpt mainly helps in non code related issues like setup issues or exploring any new syatems</t>
+  </si>
+  <si>
+    <t>I mostly use normal mode but some times i had to switch to max mode as normal mode is not able to solve the issue</t>
+  </si>
+  <si>
+    <t>To write component tests for an yet to be developed feature. As Tech design has complete details, uploaded it and cursor helped me generate tests in no time.</t>
+  </si>
+  <si>
+    <t>I use chatgpt to ask questions that are non coding related</t>
+  </si>
+  <si>
+    <t>Claude Models with Non Max mode</t>
+  </si>
+  <si>
+    <t>Keeping JIRA less complex and easy going can be one way of improving better JIRA usage</t>
+  </si>
+  <si>
+    <t>Refactoring mapper 2.0, it raised a PR in few minutes although it has not been merged and pending for review</t>
+  </si>
+  <si>
+    <t>ChatGPT is one of the best tools for research and getting broader perspective on design and overall information. It better than cursor in such areas. Definitely, chatGPT is a must tool.</t>
+  </si>
+  <si>
+    <t>Its quite good, but needs to be used with some caution for PR reviews. It can help but sometimes flags unnecessary things</t>
+  </si>
+  <si>
+    <t>Agent mode with claude sonet or gpt 5 ( till its available )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updating dates as priority </t>
+  </si>
+  <si>
+    <t>helped write scripts which will take lot of time manually</t>
+  </si>
+  <si>
+    <t>GPT will be useful to understand the overrall scenario or usecases how users will use and the new features across</t>
+  </si>
+  <si>
+    <t>Claude 4.1 / GPT5</t>
+  </si>
+  <si>
+    <t>Used cursor to develop an HTTP server which can accept multipart/form-data requests with different encodings.
+This will help us reduce the dependency on the actual application to verify multipart/form-data with encodings use-cases.
+Though multiple (refined) prompts were required, cursor did fairly well in creating the mock server.
+I'll be taking up the testing of the server.
+If everything goes well, the next task would be to create mock servers for different use cases for which we don't have the perpetual accounts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, </t>
+  </si>
+  <si>
+    <t>The cursor works well for the simple use cases but as the complexity increases more prompts are required and many a times cursor ends up doing the incorrect changes.</t>
+  </si>
+  <si>
+    <t>SathishKumar D</t>
+  </si>
+  <si>
+    <t>optimus</t>
+  </si>
+  <si>
+    <t>action was to write tcs on sso functionalities</t>
+  </si>
+  <si>
+    <t>writing test cases</t>
+  </si>
+  <si>
+    <t>Exploring / understanding existing codebase, Writing code for new features, Debugging and Fixing Bugs</t>
+  </si>
+  <si>
+    <t>cursor helped me in understanding exitsting code base and write a new code from scratch</t>
+  </si>
+  <si>
+    <t>good tool with adoption of changes features</t>
+  </si>
+  <si>
+    <t>dark mode</t>
+  </si>
+  <si>
+    <t>Updating Jira fields effectively</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recently, Dropbox account got suspended for exceeding the storage limit (270GB). As per my prompts and my instructions, With the help of Cursor, I generated a cleanup script that gave a step-by-step breakdown of the files to be deleted. Using this, I cleared multiple unwanted files created by automation test cases and freed up 270GB of space, leaving only 1.58GB used. </t>
+  </si>
+  <si>
+    <t>Will be using chatgpt for test designs, However same can be get it by cursor IDE, but I felt CHATGPT test designs are more effective.</t>
+  </si>
+  <si>
+    <t>claude-4-sonnet(MAX MODE)</t>
+  </si>
+  <si>
+    <t>Optimus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA Automation </t>
+  </si>
+  <si>
+    <t>Dev Prototype, Exploring / understanding existing codebase, Writing code for new features, Creating test cases or test scripts</t>
+  </si>
+  <si>
+    <t>Cursor helped me for setting up K8's in local with jenkins</t>
+  </si>
+  <si>
+    <t>Yes, if something we want to learn/solve/document apart from regular GIT related tasks , chatgpt is helping</t>
+  </si>
+  <si>
+    <t>Cursor saving 50% of my time for all type of Framework related tasks</t>
   </si>
 </sst>
 </file>
@@ -3019,10 +3319,10 @@
         <color rgb="FF442F65"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -3031,13 +3331,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -3132,7 +3432,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses" displayName="Form_Responses" ref="A1:AY165">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses" displayName="Form_Responses" ref="A1:AY184">
   <tableColumns count="51">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Timestamp"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="You are part of which of the following directors org"/>
@@ -3391,7 +3691,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AY165"/>
+  <dimension ref="A1:AY184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11744,7 +12044,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="1:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:50" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="4">
         <v>45881.559087615737</v>
       </c>
@@ -25442,58 +25742,2196 @@
       </c>
     </row>
     <row r="165" spans="1:50" ht="13" x14ac:dyDescent="0.15">
-      <c r="A165" s="10">
+      <c r="A165" s="7">
         <v>45882.918525543981</v>
       </c>
-      <c r="B165" s="11" t="s">
+      <c r="B165" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C165" s="11" t="s">
+      <c r="C165" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D165" s="11" t="s">
+      <c r="D165" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E165" s="11" t="s">
+      <c r="E165" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="F165" s="11">
-        <v>4</v>
-      </c>
-      <c r="G165" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="H165" s="11" t="s">
+      <c r="F165" s="8">
+        <v>4</v>
+      </c>
+      <c r="G165" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H165" s="8" t="s">
         <v>919</v>
       </c>
-      <c r="I165" s="11" t="s">
+      <c r="I165" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AP165" s="11" t="s">
+      <c r="AP165" s="8" t="s">
         <v>920</v>
       </c>
-      <c r="AQ165" s="11" t="s">
+      <c r="AQ165" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AR165" s="11" t="s">
+      <c r="AR165" s="8" t="s">
         <v>510</v>
       </c>
-      <c r="AS165" s="11" t="s">
+      <c r="AS165" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AT165" s="11" t="s">
+      <c r="AT165" s="8" t="s">
         <v>921</v>
       </c>
-      <c r="AU165" s="11" t="s">
+      <c r="AU165" s="8" t="s">
         <v>922</v>
       </c>
-      <c r="AV165" s="11" t="s">
+      <c r="AV165" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="AW165" s="11" t="s">
+      <c r="AW165" s="8" t="s">
         <v>923</v>
       </c>
-      <c r="AX165" s="11" t="s">
+      <c r="AX165" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="166" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A166" s="4">
+        <v>45883.979220069443</v>
+      </c>
+      <c r="B166" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="C166" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="D166" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E166" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="F166" s="5">
+        <v>5</v>
+      </c>
+      <c r="G166" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H166" s="5" t="s">
+        <v>925</v>
+      </c>
+      <c r="I166" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP166" s="5" t="s">
+        <v>926</v>
+      </c>
+      <c r="AQ166" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR166" s="5" t="s">
+        <v>927</v>
+      </c>
+      <c r="AS166" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT166" s="5" t="s">
+        <v>928</v>
+      </c>
+      <c r="AU166" s="5" t="s">
+        <v>929</v>
+      </c>
+      <c r="AV166" s="5" t="s">
+        <v>930</v>
+      </c>
+      <c r="AW166" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX166" s="5" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="167" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A167" s="7">
+        <v>45884.130254340278</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C167" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D167" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E167" s="8" t="s">
+        <v>932</v>
+      </c>
+      <c r="F167" s="8">
+        <v>4</v>
+      </c>
+      <c r="G167" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H167" s="8" t="s">
+        <v>933</v>
+      </c>
+      <c r="I167" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J167" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K167" s="8">
+        <v>3</v>
+      </c>
+      <c r="L167" s="8">
+        <v>5</v>
+      </c>
+      <c r="M167" s="8">
+        <v>5</v>
+      </c>
+      <c r="N167" s="8">
+        <v>5</v>
+      </c>
+      <c r="O167" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P167" s="8">
+        <v>5</v>
+      </c>
+      <c r="Q167" s="8">
+        <v>4</v>
+      </c>
+      <c r="R167" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="S167" s="8">
+        <v>4</v>
+      </c>
+      <c r="T167" s="8">
+        <v>4</v>
+      </c>
+      <c r="U167" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="V167" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="W167" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="X167" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y167" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z167" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA167" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB167" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC167" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD167" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE167" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF167" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG167" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH167" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI167" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="AJ167" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK167" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="AM167" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN167" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="AQ167" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR167" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="AS167" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT167" s="8" t="s">
+        <v>934</v>
+      </c>
+      <c r="AU167" s="8" t="s">
+        <v>935</v>
+      </c>
+      <c r="AV167" s="8" t="s">
+        <v>936</v>
+      </c>
+      <c r="AW167" s="8" t="s">
+        <v>937</v>
+      </c>
+      <c r="AX167" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="168" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A168" s="4">
+        <v>45884.161489178237</v>
+      </c>
+      <c r="B168" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D168" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E168" s="5" t="s">
+        <v>932</v>
+      </c>
+      <c r="F168" s="5">
+        <v>5</v>
+      </c>
+      <c r="G168" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H168" s="5" t="s">
+        <v>938</v>
+      </c>
+      <c r="I168" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J168" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K168" s="5">
+        <v>4</v>
+      </c>
+      <c r="L168" s="5">
+        <v>5</v>
+      </c>
+      <c r="M168" s="5">
+        <v>5</v>
+      </c>
+      <c r="N168" s="5">
+        <v>5</v>
+      </c>
+      <c r="O168" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P168" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q168" s="5">
+        <v>5</v>
+      </c>
+      <c r="R168" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="S168" s="5">
+        <v>5</v>
+      </c>
+      <c r="T168" s="5">
+        <v>5</v>
+      </c>
+      <c r="U168" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V168" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W168" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="X168" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y168" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z168" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="AA168" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB168" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC168" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD168" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE168" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF168" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG168" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="AH168" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI168" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="AJ168" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="AK168" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM168" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN168" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ168" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR168" s="5" t="s">
+        <v>939</v>
+      </c>
+      <c r="AS168" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT168" s="5" t="s">
+        <v>940</v>
+      </c>
+      <c r="AU168" s="5" t="s">
+        <v>941</v>
+      </c>
+      <c r="AV168" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW168" s="5" t="s">
+        <v>942</v>
+      </c>
+      <c r="AX168" s="5" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="169" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A169" s="7">
+        <v>45884.640528738426</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C169" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D169" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I169" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J169" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K169" s="8">
+        <v>5</v>
+      </c>
+      <c r="L169" s="8">
+        <v>5</v>
+      </c>
+      <c r="M169" s="8">
+        <v>5</v>
+      </c>
+      <c r="N169" s="8">
+        <v>5</v>
+      </c>
+      <c r="O169" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P169" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q169" s="8">
+        <v>4</v>
+      </c>
+      <c r="R169" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="S169" s="8">
+        <v>4</v>
+      </c>
+      <c r="T169" s="8">
+        <v>4</v>
+      </c>
+      <c r="U169" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="V169" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="W169" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="X169" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y169" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z169" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA169" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB169" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC169" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD169" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE169" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF169" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG169" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH169" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI169" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ169" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="AK169" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="AM169" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN169" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="AO169" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="AQ169" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR169" s="8" t="s">
+        <v>944</v>
+      </c>
+      <c r="AS169" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT169" s="8" t="s">
+        <v>945</v>
+      </c>
+      <c r="AU169" s="8" t="s">
+        <v>946</v>
+      </c>
+      <c r="AV169" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW169" s="8" t="s">
+        <v>947</v>
+      </c>
+      <c r="AX169" s="8" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="170" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A170" s="4">
+        <v>45885.436984826389</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C170" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="D170" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E170" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="F170" s="5">
+        <v>5</v>
+      </c>
+      <c r="G170" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H170" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="I170" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J170" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K170" s="5">
+        <v>4</v>
+      </c>
+      <c r="L170" s="5">
+        <v>4</v>
+      </c>
+      <c r="M170" s="5">
+        <v>4</v>
+      </c>
+      <c r="N170" s="5">
+        <v>4</v>
+      </c>
+      <c r="O170" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P170" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q170" s="5">
+        <v>4</v>
+      </c>
+      <c r="R170" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="S170" s="5">
+        <v>4</v>
+      </c>
+      <c r="T170" s="5">
+        <v>4</v>
+      </c>
+      <c r="U170" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V170" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W170" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="X170" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y170" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z170" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA170" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB170" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC170" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD170" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE170" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF170" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG170" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH170" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI170" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="AJ170" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK170" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL170" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM170" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN170" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ170" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR170" s="5" t="s">
+        <v>632</v>
+      </c>
+      <c r="AS170" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT170" s="5" t="s">
+        <v>950</v>
+      </c>
+      <c r="AU170" s="5" t="s">
+        <v>951</v>
+      </c>
+      <c r="AV170" s="5" t="s">
+        <v>952</v>
+      </c>
+      <c r="AW170" s="5" t="s">
+        <v>953</v>
+      </c>
+      <c r="AX170" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="171" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A171" s="7">
+        <v>45885.649163020833</v>
+      </c>
+      <c r="B171" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C171" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D171" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I171" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J171" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K171" s="8">
+        <v>4</v>
+      </c>
+      <c r="L171" s="8">
+        <v>4</v>
+      </c>
+      <c r="M171" s="8">
+        <v>5</v>
+      </c>
+      <c r="N171" s="8">
+        <v>5</v>
+      </c>
+      <c r="O171" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="P171" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q171" s="8">
+        <v>4</v>
+      </c>
+      <c r="R171" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="S171" s="8">
+        <v>4</v>
+      </c>
+      <c r="T171" s="8">
+        <v>4</v>
+      </c>
+      <c r="U171" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="V171" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="W171" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="X171" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y171" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z171" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA171" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB171" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC171" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD171" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE171" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF171" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG171" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH171" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="AI171" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="AJ171" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK171" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="AM171" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN171" s="8" t="s">
+        <v>954</v>
+      </c>
+      <c r="AO171" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ171" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR171" s="8" t="s">
+        <v>955</v>
+      </c>
+      <c r="AS171" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT171" s="8" t="s">
+        <v>956</v>
+      </c>
+      <c r="AU171" s="8" t="s">
+        <v>957</v>
+      </c>
+      <c r="AV171" s="8" t="s">
+        <v>958</v>
+      </c>
+      <c r="AW171" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="AX171" s="8" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="172" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A172" s="4">
+        <v>45887.364872418984</v>
+      </c>
+      <c r="B172" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C172" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D172" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="I172" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP172" s="5" t="s">
+        <v>961</v>
+      </c>
+      <c r="AQ172" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR172" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="AS172" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="AT172" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="AU172" s="5" t="s">
+        <v>964</v>
+      </c>
+      <c r="AV172" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="AW172" s="5" t="s">
+        <v>966</v>
+      </c>
+      <c r="AX172" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="173" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A173" s="7">
+        <v>45887.372886597223</v>
+      </c>
+      <c r="B173" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C173" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D173" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="I173" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP173" s="8" t="s">
+        <v>967</v>
+      </c>
+      <c r="AQ173" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR173" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="AS173" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT173" s="8" t="s">
+        <v>968</v>
+      </c>
+      <c r="AU173" s="8" t="s">
+        <v>969</v>
+      </c>
+      <c r="AV173" s="8" t="s">
+        <v>970</v>
+      </c>
+      <c r="AW173" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX173" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="174" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A174" s="4">
+        <v>45887.403524768517</v>
+      </c>
+      <c r="B174" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C174" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D174" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E174" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F174" s="5">
+        <v>5</v>
+      </c>
+      <c r="G174" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H174" s="5" t="s">
+        <v>971</v>
+      </c>
+      <c r="I174" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J174" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K174" s="5">
+        <v>5</v>
+      </c>
+      <c r="L174" s="5">
+        <v>5</v>
+      </c>
+      <c r="M174" s="5">
+        <v>5</v>
+      </c>
+      <c r="N174" s="5">
+        <v>5</v>
+      </c>
+      <c r="O174" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P174" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q174" s="5">
+        <v>5</v>
+      </c>
+      <c r="R174" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="S174" s="5">
+        <v>5</v>
+      </c>
+      <c r="T174" s="5">
+        <v>5</v>
+      </c>
+      <c r="U174" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V174" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W174" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="X174" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y174" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z174" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA174" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB174" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC174" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD174" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE174" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF174" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG174" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH174" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI174" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="AJ174" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK174" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM174" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN174" s="5" t="s">
+        <v>652</v>
+      </c>
+      <c r="AQ174" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR174" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="AS174" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT174" s="5" t="s">
+        <v>972</v>
+      </c>
+      <c r="AU174" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="AV174" s="5" t="s">
+        <v>974</v>
+      </c>
+      <c r="AW174" s="5" t="s">
+        <v>672</v>
+      </c>
+      <c r="AX174" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="175" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A175" s="7">
+        <v>45887.407632569448</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C175" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D175" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E175" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="F175" s="8">
+        <v>4</v>
+      </c>
+      <c r="G175" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I175" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J175" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K175" s="8">
+        <v>4</v>
+      </c>
+      <c r="L175" s="8">
+        <v>4</v>
+      </c>
+      <c r="M175" s="8">
+        <v>4</v>
+      </c>
+      <c r="N175" s="8">
+        <v>4</v>
+      </c>
+      <c r="O175" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P175" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q175" s="8">
+        <v>4</v>
+      </c>
+      <c r="R175" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="S175" s="8">
+        <v>4</v>
+      </c>
+      <c r="T175" s="8">
+        <v>4</v>
+      </c>
+      <c r="U175" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="V175" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="W175" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="X175" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y175" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z175" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA175" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB175" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC175" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD175" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE175" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF175" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG175" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH175" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="AI175" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ175" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK175" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM175" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN175" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ175" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR175" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="AS175" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT175" s="8" t="s">
+        <v>975</v>
+      </c>
+      <c r="AU175" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AV175" s="8" t="s">
+        <v>976</v>
+      </c>
+      <c r="AW175" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="AX175" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="176" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A176" s="4">
+        <v>45887.410724467598</v>
+      </c>
+      <c r="B176" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C176" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D176" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="I176" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ176" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR176" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS176" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT176" s="5" t="s">
+        <v>977</v>
+      </c>
+      <c r="AU176" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="AV176" s="5" t="s">
+        <v>979</v>
+      </c>
+      <c r="AW176" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="AX176" s="5" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="177" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A177" s="7">
+        <v>45887.433398842593</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C177" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="D177" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E177" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="F177" s="8">
+        <v>4</v>
+      </c>
+      <c r="G177" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H177" s="8" t="s">
+        <v>981</v>
+      </c>
+      <c r="I177" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J177" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K177" s="8">
+        <v>5</v>
+      </c>
+      <c r="M177" s="8">
+        <v>4</v>
+      </c>
+      <c r="N177" s="8">
+        <v>5</v>
+      </c>
+      <c r="O177" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P177" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q177" s="8">
+        <v>4</v>
+      </c>
+      <c r="R177" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="S177" s="8">
+        <v>5</v>
+      </c>
+      <c r="T177" s="8">
+        <v>5</v>
+      </c>
+      <c r="U177" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="V177" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="W177" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="X177" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y177" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z177" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="AA177" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB177" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC177" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD177" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE177" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF177" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="AG177" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH177" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI177" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="AJ177" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="AK177" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL177" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM177" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN177" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AO177" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ177" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR177" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="AS177" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT177" s="8" t="s">
+        <v>982</v>
+      </c>
+      <c r="AU177" s="8" t="s">
+        <v>983</v>
+      </c>
+      <c r="AV177" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW177" s="8" t="s">
+        <v>984</v>
+      </c>
+      <c r="AX177" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="178" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A178" s="4">
+        <v>45887.450998310189</v>
+      </c>
+      <c r="B178" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C178" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D178" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="I178" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J178" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K178" s="5">
+        <v>4</v>
+      </c>
+      <c r="L178" s="5">
+        <v>4</v>
+      </c>
+      <c r="M178" s="5">
+        <v>4</v>
+      </c>
+      <c r="N178" s="5">
+        <v>4</v>
+      </c>
+      <c r="O178" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="P178" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q178" s="5">
+        <v>4</v>
+      </c>
+      <c r="R178" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="S178" s="5">
+        <v>4</v>
+      </c>
+      <c r="T178" s="5">
+        <v>4</v>
+      </c>
+      <c r="U178" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V178" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W178" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="X178" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y178" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z178" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA178" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB178" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC178" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD178" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE178" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF178" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG178" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH178" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI178" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="AJ178" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK178" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM178" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN178" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO178" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ178" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR178" s="5" t="s">
+        <v>955</v>
+      </c>
+      <c r="AS178" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT178" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="AU178" s="5" t="s">
+        <v>986</v>
+      </c>
+      <c r="AV178" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="AW178" s="5" t="s">
+        <v>987</v>
+      </c>
+      <c r="AX178" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="179" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A179" s="7">
+        <v>45887.456081712968</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C179" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D179" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E179" s="8" t="s">
+        <v>630</v>
+      </c>
+      <c r="F179" s="8">
+        <v>4</v>
+      </c>
+      <c r="G179" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H179" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I179" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J179" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K179" s="8">
+        <v>4</v>
+      </c>
+      <c r="L179" s="8">
+        <v>5</v>
+      </c>
+      <c r="M179" s="8">
+        <v>4</v>
+      </c>
+      <c r="N179" s="8">
+        <v>5</v>
+      </c>
+      <c r="O179" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P179" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q179" s="8">
+        <v>4</v>
+      </c>
+      <c r="R179" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="S179" s="8">
+        <v>3</v>
+      </c>
+      <c r="T179" s="8">
+        <v>4</v>
+      </c>
+      <c r="U179" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="V179" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="W179" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="X179" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y179" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z179" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA179" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB179" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC179" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD179" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE179" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF179" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG179" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH179" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI179" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="AJ179" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK179" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM179" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN179" s="8" t="s">
+        <v>988</v>
+      </c>
+      <c r="AQ179" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR179" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="AS179" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT179" s="8" t="s">
+        <v>989</v>
+      </c>
+      <c r="AU179" s="8" t="s">
+        <v>990</v>
+      </c>
+      <c r="AV179" s="8" t="s">
+        <v>991</v>
+      </c>
+      <c r="AW179" s="8" t="s">
+        <v>992</v>
+      </c>
+      <c r="AX179" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="180" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A180" s="4">
+        <v>45887.45851950231</v>
+      </c>
+      <c r="B180" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C180" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D180" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E180" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F180" s="5">
+        <v>4</v>
+      </c>
+      <c r="G180" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H180" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="I180" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J180" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K180" s="5">
+        <v>4</v>
+      </c>
+      <c r="L180" s="5">
+        <v>4</v>
+      </c>
+      <c r="M180" s="5">
+        <v>4</v>
+      </c>
+      <c r="N180" s="5">
+        <v>4</v>
+      </c>
+      <c r="O180" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P180" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q180" s="5">
+        <v>4</v>
+      </c>
+      <c r="R180" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="S180" s="5">
+        <v>4</v>
+      </c>
+      <c r="T180" s="5">
+        <v>4</v>
+      </c>
+      <c r="U180" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V180" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W180" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="X180" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y180" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z180" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA180" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB180" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC180" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD180" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE180" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF180" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG180" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH180" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI180" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ180" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="AK180" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM180" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN180" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="AQ180" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR180" s="5" t="s">
+        <v>632</v>
+      </c>
+      <c r="AS180" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT180" s="5" t="s">
+        <v>994</v>
+      </c>
+      <c r="AU180" s="5" t="s">
+        <v>995</v>
+      </c>
+      <c r="AV180" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="AW180" s="5" t="s">
+        <v>996</v>
+      </c>
+      <c r="AX180" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="181" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A181" s="7">
+        <v>45887.45917318287</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C181" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="D181" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E181" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="F181" s="8">
+        <v>4</v>
+      </c>
+      <c r="G181" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I181" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J181" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K181" s="8">
+        <v>4</v>
+      </c>
+      <c r="L181" s="8">
+        <v>4</v>
+      </c>
+      <c r="M181" s="8">
+        <v>4</v>
+      </c>
+      <c r="N181" s="8">
+        <v>4</v>
+      </c>
+      <c r="O181" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P181" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q181" s="8">
+        <v>4</v>
+      </c>
+      <c r="R181" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="S181" s="8">
+        <v>4</v>
+      </c>
+      <c r="T181" s="8">
+        <v>4</v>
+      </c>
+      <c r="U181" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="V181" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="W181" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="X181" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y181" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z181" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA181" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB181" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC181" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD181" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE181" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF181" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG181" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH181" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI181" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="AJ181" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK181" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL181" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM181" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN181" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AO181" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ181" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR181" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="AS181" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AT181" s="8" t="s">
+        <v>997</v>
+      </c>
+      <c r="AU181" s="8" t="s">
+        <v>998</v>
+      </c>
+      <c r="AV181" s="8" t="s">
+        <v>999</v>
+      </c>
+      <c r="AW181" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX181" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="182" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A182" s="4">
+        <v>45887.471067592589</v>
+      </c>
+      <c r="B182" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C182" s="5" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D182" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E182" s="5" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F182" s="5">
+        <v>4</v>
+      </c>
+      <c r="G182" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H182" s="5" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I182" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP182" s="5" t="s">
+        <v>1003</v>
+      </c>
+      <c r="AQ182" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR182" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="AS182" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT182" s="5" t="s">
+        <v>1005</v>
+      </c>
+      <c r="AU182" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV182" s="5" t="s">
+        <v>1006</v>
+      </c>
+      <c r="AW182" s="5" t="s">
+        <v>1007</v>
+      </c>
+      <c r="AX182" s="5" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="183" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A183" s="7">
+        <v>45887.48655587963</v>
+      </c>
+      <c r="B183" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C183" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D183" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E183" s="8" t="s">
+        <v>503</v>
+      </c>
+      <c r="F183" s="8">
+        <v>5</v>
+      </c>
+      <c r="G183" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H183" s="8" t="s">
+        <v>1008</v>
+      </c>
+      <c r="I183" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J183" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K183" s="8">
+        <v>4</v>
+      </c>
+      <c r="L183" s="8">
+        <v>5</v>
+      </c>
+      <c r="M183" s="8">
+        <v>5</v>
+      </c>
+      <c r="N183" s="8">
+        <v>5</v>
+      </c>
+      <c r="O183" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P183" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q183" s="8">
+        <v>5</v>
+      </c>
+      <c r="R183" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="S183" s="8">
+        <v>5</v>
+      </c>
+      <c r="T183" s="8">
+        <v>3</v>
+      </c>
+      <c r="U183" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="V183" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="W183" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="X183" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y183" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z183" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA183" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB183" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC183" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD183" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE183" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF183" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG183" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH183" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="AI183" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ183" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="AK183" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="AL183" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM183" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN183" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AO183" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ183" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR183" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="AS183" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT183" s="8" t="s">
+        <v>1009</v>
+      </c>
+      <c r="AU183" s="8" t="s">
+        <v>1010</v>
+      </c>
+      <c r="AV183" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW183" s="8" t="s">
+        <v>1011</v>
+      </c>
+      <c r="AX183" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="184" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A184" s="10">
+        <v>45887.601201527781</v>
+      </c>
+      <c r="B184" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C184" s="11" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D184" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E184" s="11" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F184" s="11">
+        <v>4</v>
+      </c>
+      <c r="G184" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I184" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP184" s="11" t="s">
+        <v>1013</v>
+      </c>
+      <c r="AQ184" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR184" s="11" t="s">
+        <v>1014</v>
+      </c>
+      <c r="AS184" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT184" s="11" t="s">
+        <v>1015</v>
+      </c>
+      <c r="AU184" s="11" t="s">
+        <v>1016</v>
+      </c>
+      <c r="AV184" s="11" t="s">
+        <v>1017</v>
+      </c>
+      <c r="AW184" s="11" t="s">
+        <v>704</v>
+      </c>
+      <c r="AX184" s="11" t="s">
         <v>104</v>
       </c>
     </row>
@@ -25503,4 +27941,23 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="38" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix response count discrepancy - clarify total vs question-specific counts
- Updated 'Total Responses by Release' chart title to 'Total Survey Responses by Release'
- Added explanatory text: 'Shows total number of people who completed the survey (may not have answered every question)'
- Enhanced hover tooltips in TrendChart to clearly show 'Question-specific responses:'
- Added explanatory text above trend charts: 'Hover over data points to see question-specific response counts (excludes people who skipped this question)'
- Added clarification in Director Analysis: 'Shows responses from [Director]'s team only. Hover over data points to see counts.'

Resolves user confusion between:
- Total survey responses (206 for August 2025)
- Question-specific responses (171 for August 2025 'Rate Release Overall' question)
</commit_message>
<xml_diff>
--- a/Retrospectives/August 2025 Release Retrospective (Responses).xlsx
+++ b/Retrospectives/August 2025 Release Retrospective (Responses).xlsx
@@ -8,21 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajendran/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF046A68-53D1-EB49-870F-4A3B1EAB29A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E8F6493-C3FF-6D4F-9F76-6957D038EF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
     <sheet name="Pivot Table 1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form Responses 1'!$A$1:$AY$207</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6279" uniqueCount="1018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6897" uniqueCount="1122">
   <si>
     <t>Timestamp</t>
   </si>
@@ -3139,6 +3155,323 @@
   </si>
   <si>
     <t>Cursor saving 50% of my time for all type of Framework related tasks</t>
+  </si>
+  <si>
+    <t>We are not involved in release directly as we are part of the core automation team, rather we help QA and Dev to facilitate release.</t>
+  </si>
+  <si>
+    <t>We were maintaining the automation frameworks on which QA and Dev run their tests</t>
+  </si>
+  <si>
+    <t>It helped me actually identifying the existing issues in framework and how can we increase the readability and maintainability of the existing code.</t>
+  </si>
+  <si>
+    <t>Yes I use chat gpt also, if we want some general information on any specific topic then i think chat gpt gives better results than cursor</t>
+  </si>
+  <si>
+    <t>I have faced sometime the situation when it gets stuck in loop and remain stuck for hours and do not give the result</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
+  </si>
+  <si>
+    <t>To give me the list of trackers assigned to me with some specific names and to fetch the git PRs on them</t>
+  </si>
+  <si>
+    <t>Yes, ChatGPT is good in certain things like generating images with explanations, and also we use it as second opinion and for catching the mistakes by Cursor</t>
+  </si>
+  <si>
+    <t>Max Mode without Auto</t>
+  </si>
+  <si>
+    <t>Since I belong to the Automation Team, we are not directly involved in feature development but play a key role in providing framework support to both QA and Development teams. We have also extended Canary support for REST services as well as Playwright triggers. For the August release, we successfully delivered these enhancements for both IAQA and Staging environments.</t>
+  </si>
+  <si>
+    <t>One interesting use case where Cursor really helped me was in understanding Contract Testing efficiency. With its assistance, I was able to quickly grasp complex code flows that would have otherwise taken much longer to break down manually. Cursor not only simplified the learning process but also enabled me to make meaningful additions and improvements in the codebase with confidence.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, ChatGPT adds value beyond an AI-enabled IDE. I use it for , Quickly clarifying complex concepts.Drafting clear communication or documentation. Exploring ideas and best practices outside of pure coding.
+</t>
+  </si>
+  <si>
+    <t>Cursor has been very helpful in understanding complex code, improving contract testing efficiency, and speeding up development by providing accurate context-aware suggestions.</t>
+  </si>
+  <si>
+    <t>I prefer using Cursor in Chat mode, as it helps me quickly understand complex code, clarify logic, and explore solutions interactively.</t>
+  </si>
+  <si>
+    <t>Handling new feature and adapting it</t>
+  </si>
+  <si>
+    <t>handling automation framework</t>
+  </si>
+  <si>
+    <t>To make code more deliverable</t>
+  </si>
+  <si>
+    <t>Privacy</t>
+  </si>
+  <si>
+    <t>Writing code for new features</t>
+  </si>
+  <si>
+    <t>In IA shopify repo for Deprecated changes, Without change old code added new changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It's best platform, We are increased productivity </t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI Automation stability tasks </t>
+  </si>
+  <si>
+    <t>Exploring / understanding existing codebase, Review PRs, Writing Unit tests, Creating test cases or test scripts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Able to modify reports upload to report portal , with in a short duration </t>
+  </si>
+  <si>
+    <t>Yes, I use ChatGPT beyond my IDE for quick problem-solving, brainstorming ideas, and clarifying complex concepts.</t>
+  </si>
+  <si>
+    <t>Cursor is an excellent and  great for fast, AI-assisted coding with in-context suggestions. It could improve with deeper project-wide understanding and smarter refactoring support</t>
+  </si>
+  <si>
+    <t>I prefer Chat mode for explanations and brainstorming, and Edit mode when I need direct code modifications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes </t>
+  </si>
+  <si>
+    <t>allocation of tasks as per the band width and based on resource availability</t>
+  </si>
+  <si>
+    <t>enhancement of the automation framework</t>
+  </si>
+  <si>
+    <t>with a single prompt we can perform git actions like commit abort, raise a pull request etc</t>
+  </si>
+  <si>
+    <t>It helps understanding the framework and code base very easily without the need of Kt's</t>
+  </si>
+  <si>
+    <t>Cursor is a great stuff to use but sometimes it is hallucinating and providing the unnecessary changes to the files</t>
+  </si>
+  <si>
+    <t>Yes. The support can be further improved over slack like by providing weekly or day to day tips etc</t>
+  </si>
+  <si>
+    <t>We stabilized the suites</t>
+  </si>
+  <si>
+    <t>Writing Testcases and sharing knowledge to new joiners</t>
+  </si>
+  <si>
+    <t>Github,Shopify,Attlasian MCP are very useful</t>
+  </si>
+  <si>
+    <t>velocity of writing TC is increased</t>
+  </si>
+  <si>
+    <t>Analyse the bug and details on fixing and generating the test cases</t>
+  </si>
+  <si>
+    <t>Yes, for getting details understanding on any topics</t>
+  </si>
+  <si>
+    <t>It helped me identify all the places where the setting is having an effect. Using that information, I updated the dependent areas accordingly.</t>
+  </si>
+  <si>
+    <t>Yes — I use ChatGPT for quick explanations, brainstorming, and drafting, beyond just coding in the IDE.</t>
+  </si>
+  <si>
+    <t>Claude 4</t>
+  </si>
+  <si>
+    <t>Different action items are decided based on the sprint retro and discussion. We discuss what can be improved and take action items on individual and team, e.g. code review should be given to reviewer by Friday EOD so that the reviews can be addressed and that particular item should be merged and completed within the sprint.</t>
+  </si>
+  <si>
+    <t>Although we can't rely completely on cursor but it helps to identify what code does and fix test cases, find possible leaks/issues.</t>
+  </si>
+  <si>
+    <t>Yes, IDE is good to work with during writing and debugging code but ChatGPT is good with alot of other tasks such as data generation for test cases, writing queries, researching etc.</t>
+  </si>
+  <si>
+    <t>We need to have a detailed document on the best practices, uses, features and how to enable these features.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, it can be improved by automating the process to give different access and maintain the best practices and guidelines for use. </t>
+  </si>
+  <si>
+    <t>Helped me write skeletons of code once I explained the basic requirements and add the tests as well. Both functional and integration tests.</t>
+  </si>
+  <si>
+    <t>Chatgpt definitely has value in addition to using an AI based IDE, because in cases like building snowflake splunk queries, we're able to make use of gpt. Also something out of direct code context is helpful via chatgpt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cursor is a good tool to write test-cases explain code and even write code skeletons. It does redundant jobs quickly and saves time. Also it helps identify places which we're probably looking for for code to be added. </t>
+  </si>
+  <si>
+    <t>Cursor help in finding the loop holes which we are missing that will break the functionality in future which we are currently implementing</t>
+  </si>
+  <si>
+    <t>I don't have access to chatGPT</t>
+  </si>
+  <si>
+    <t>its good, helped in understanding the code</t>
+  </si>
+  <si>
+    <t>claude 3.7 sonnet(max mode)</t>
+  </si>
+  <si>
+    <t>No action items</t>
+  </si>
+  <si>
+    <t>If we give the tech design doc, its implementing the code very well with out any bugs</t>
+  </si>
+  <si>
+    <t>While working on tech design, chatGPT is very helpful rather than cursor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It increased productivity a lot. </t>
+  </si>
+  <si>
+    <t>cloaude sonnet 4.0</t>
+  </si>
+  <si>
+    <t>Give the test design and ask to code</t>
+  </si>
+  <si>
+    <t>yes, useful for deep research</t>
+  </si>
+  <si>
+    <t>its very valuable</t>
+  </si>
+  <si>
+    <t>Chakra</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>there are few way I used cursor for
+1. to generate sequence diagram
+2. help to document any low level tech design
+3. implement code changes by providing the TD(relevant section)</t>
+  </si>
+  <si>
+    <t>minimal usages when checking for some high level design changes/suggestion</t>
+  </si>
+  <si>
+    <t>some times the time we spent in explaining the task and after it completes the task reviewing and updating it is 2X or 3X</t>
+  </si>
+  <si>
+    <t>cloud-sonnet-4</t>
+  </si>
+  <si>
+    <t>Release management and QA activities</t>
+  </si>
+  <si>
+    <t>Review PRs</t>
+  </si>
+  <si>
+    <t>Identify the hardcoded locators in the code, for which I was dependent on team to do the analysis and provide</t>
+  </si>
+  <si>
+    <t>Using chatGPT for anything and everything for my day-to-day activities</t>
+  </si>
+  <si>
+    <t>get design feedbacks before sprint</t>
+  </si>
+  <si>
+    <t>its help find impact on the new changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes chatgpt is go to for research and quickly identifying gaps </t>
+  </si>
+  <si>
+    <t>Ask,Tab</t>
+  </si>
+  <si>
+    <t>We would need proper backlog/roadmap</t>
+  </si>
+  <si>
+    <t>Identifying the potential expected bugs, automating the test cases, report validations using cursor.</t>
+  </si>
+  <si>
+    <t>I use ChatGPT for a broader range of activities</t>
+  </si>
+  <si>
+    <t>This has been the most effective tool in supporting my day-to-day activities, and I’m keen to explore it further.</t>
+  </si>
+  <si>
+    <t>I primarily use Edit Mode, with Chat Mode as my secondary preference</t>
+  </si>
+  <si>
+    <t>Getting enough support</t>
+  </si>
+  <si>
+    <t>Explaining code base</t>
+  </si>
+  <si>
+    <t>Yes, Creating automation tests and exploring product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is inconsistent. Responses are differ every time. </t>
+  </si>
+  <si>
+    <t>backlog automation tasks</t>
+  </si>
+  <si>
+    <t>Create test scripts</t>
+  </si>
+  <si>
+    <t>it's good so far, helping for adding test scripts quickly</t>
+  </si>
+  <si>
+    <t>Chat and Edit Mode</t>
+  </si>
+  <si>
+    <t>So far good</t>
+  </si>
+  <si>
+    <t>Suite stabilization</t>
+  </si>
+  <si>
+    <t>better communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">writing refrenced test cases that will help us to save a lot of time </t>
+  </si>
+  <si>
+    <t>to get the proumpt for the cursor</t>
+  </si>
+  <si>
+    <t>claude 4</t>
+  </si>
+  <si>
+    <t>Tetris(E2E)</t>
+  </si>
+  <si>
+    <t>Drive the feedback to scrum teams through right channel to avoid any miscommunications.
+Epic testing ownership lies soley to Scrum team.</t>
+  </si>
+  <si>
+    <t>Improving my k6 tool</t>
+  </si>
+  <si>
+    <t>To perform poc on any item, its uefull</t>
+  </si>
+  <si>
+    <t>its great</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -3319,10 +3652,10 @@
         <color rgb="FF442F65"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -3331,13 +3664,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -3348,7 +3681,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3383,6 +3716,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3432,7 +3767,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses" displayName="Form_Responses" ref="A1:AY184">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses" displayName="Form_Responses" ref="A1:AY207">
+  <autoFilter ref="A1:AY207" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="51">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Timestamp"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="You are part of which of the following directors org"/>
@@ -3691,7 +4027,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AY184"/>
+  <dimension ref="A1:AY207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -27883,56 +28219,2370 @@
       </c>
     </row>
     <row r="184" spans="1:50" ht="13" x14ac:dyDescent="0.15">
-      <c r="A184" s="10">
+      <c r="A184" s="4">
         <v>45887.601201527781</v>
       </c>
-      <c r="B184" s="11" t="s">
+      <c r="B184" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C184" s="11" t="s">
+      <c r="C184" s="5" t="s">
         <v>1000</v>
       </c>
-      <c r="D184" s="11" t="s">
+      <c r="D184" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E184" s="11" t="s">
+      <c r="E184" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="F184" s="11">
-        <v>4</v>
-      </c>
-      <c r="G184" s="11" t="s">
+      <c r="F184" s="5">
+        <v>4</v>
+      </c>
+      <c r="G184" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="I184" s="11" t="s">
+      <c r="I184" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AP184" s="11" t="s">
+      <c r="AP184" s="5" t="s">
         <v>1013</v>
       </c>
-      <c r="AQ184" s="11" t="s">
+      <c r="AQ184" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AR184" s="11" t="s">
+      <c r="AR184" s="5" t="s">
         <v>1014</v>
       </c>
-      <c r="AS184" s="11" t="s">
+      <c r="AS184" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AT184" s="11" t="s">
+      <c r="AT184" s="5" t="s">
         <v>1015</v>
       </c>
-      <c r="AU184" s="11" t="s">
+      <c r="AU184" s="5" t="s">
         <v>1016</v>
       </c>
-      <c r="AV184" s="11" t="s">
+      <c r="AV184" s="5" t="s">
         <v>1017</v>
       </c>
-      <c r="AW184" s="11" t="s">
+      <c r="AW184" s="5" t="s">
         <v>704</v>
       </c>
-      <c r="AX184" s="11" t="s">
+      <c r="AX184" s="5" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="185" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A185" s="7">
+        <v>45887.631980972219</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C185" s="8" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D185" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E185" s="8" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F185" s="8">
+        <v>5</v>
+      </c>
+      <c r="G185" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H185" s="8" t="s">
+        <v>1018</v>
+      </c>
+      <c r="I185" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP185" s="8" t="s">
+        <v>1019</v>
+      </c>
+      <c r="AQ185" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR185" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="AS185" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="AT185" s="8" t="s">
+        <v>1020</v>
+      </c>
+      <c r="AU185" s="8" t="s">
+        <v>1021</v>
+      </c>
+      <c r="AV185" s="8" t="s">
+        <v>1022</v>
+      </c>
+      <c r="AW185" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="AX185" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="186" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A186" s="4">
+        <v>45887.647940266208</v>
+      </c>
+      <c r="B186" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C186" s="5" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D186" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E186" s="5" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F186" s="5">
+        <v>5</v>
+      </c>
+      <c r="G186" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H186" s="5" t="s">
+        <v>1023</v>
+      </c>
+      <c r="I186" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ186" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR186" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="AS186" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT186" s="5" t="s">
+        <v>1024</v>
+      </c>
+      <c r="AU186" s="5" t="s">
+        <v>1025</v>
+      </c>
+      <c r="AV186" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AW186" s="5" t="s">
+        <v>1026</v>
+      </c>
+      <c r="AX186" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="187" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A187" s="7">
+        <v>45887.657534409722</v>
+      </c>
+      <c r="B187" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C187" s="8" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D187" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E187" s="8" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F187" s="8">
+        <v>5</v>
+      </c>
+      <c r="G187" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H187" s="8" t="s">
+        <v>1027</v>
+      </c>
+      <c r="I187" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP187" s="8" t="s">
+        <v>1027</v>
+      </c>
+      <c r="AQ187" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR187" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="AS187" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="AT187" s="8" t="s">
+        <v>1028</v>
+      </c>
+      <c r="AU187" s="8" t="s">
+        <v>1029</v>
+      </c>
+      <c r="AV187" s="8" t="s">
+        <v>1030</v>
+      </c>
+      <c r="AW187" s="8" t="s">
+        <v>1031</v>
+      </c>
+      <c r="AX187" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="188" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A188" s="4">
+        <v>45887.658242303238</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C188" s="5" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D188" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E188" s="5" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F188" s="5">
+        <v>5</v>
+      </c>
+      <c r="G188" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H188" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="I188" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP188" s="5" t="s">
+        <v>1033</v>
+      </c>
+      <c r="AQ188" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR188" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="AS188" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT188" s="5" t="s">
+        <v>1034</v>
+      </c>
+      <c r="AU188" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AV188" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="AW188" s="5" t="s">
+        <v>1035</v>
+      </c>
+      <c r="AX188" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="189" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A189" s="7">
+        <v>45887.660893622684</v>
+      </c>
+      <c r="B189" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C189" s="8" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D189" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E189" s="8" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F189" s="8">
+        <v>5</v>
+      </c>
+      <c r="G189" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H189" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I189" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ189" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR189" s="8" t="s">
+        <v>1036</v>
+      </c>
+      <c r="AS189" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT189" s="8" t="s">
+        <v>1037</v>
+      </c>
+      <c r="AU189" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AV189" s="8" t="s">
+        <v>1038</v>
+      </c>
+      <c r="AW189" s="8" t="s">
+        <v>1039</v>
+      </c>
+      <c r="AX189" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="190" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A190" s="4">
+        <v>45887.674353055554</v>
+      </c>
+      <c r="B190" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C190" s="5" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D190" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E190" s="5" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F190" s="5">
+        <v>5</v>
+      </c>
+      <c r="G190" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H190" s="5" t="s">
+        <v>1040</v>
+      </c>
+      <c r="I190" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP190" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ190" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR190" s="5" t="s">
+        <v>1041</v>
+      </c>
+      <c r="AS190" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT190" s="5" t="s">
+        <v>1042</v>
+      </c>
+      <c r="AU190" s="5" t="s">
+        <v>1043</v>
+      </c>
+      <c r="AV190" s="5" t="s">
+        <v>1044</v>
+      </c>
+      <c r="AW190" s="5" t="s">
+        <v>1045</v>
+      </c>
+      <c r="AX190" s="5" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="191" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A191" s="7">
+        <v>45887.676318877318</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C191" s="8" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D191" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E191" s="8" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F191" s="8">
+        <v>4</v>
+      </c>
+      <c r="G191" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H191" s="8" t="s">
+        <v>1047</v>
+      </c>
+      <c r="I191" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP191" s="8" t="s">
+        <v>1048</v>
+      </c>
+      <c r="AQ191" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR191" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="AS191" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="AT191" s="8" t="s">
+        <v>1049</v>
+      </c>
+      <c r="AU191" s="8" t="s">
+        <v>1050</v>
+      </c>
+      <c r="AV191" s="8" t="s">
+        <v>1051</v>
+      </c>
+      <c r="AW191" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX191" s="8" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="192" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A192" s="4">
+        <v>45887.70201256944</v>
+      </c>
+      <c r="B192" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C192" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D192" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E192" s="5" t="s">
+        <v>853</v>
+      </c>
+      <c r="F192" s="5">
+        <v>5</v>
+      </c>
+      <c r="G192" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H192" s="5" t="s">
+        <v>1053</v>
+      </c>
+      <c r="I192" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP192" s="5" t="s">
+        <v>1054</v>
+      </c>
+      <c r="AQ192" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR192" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="AS192" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="AT192" s="5" t="s">
+        <v>1055</v>
+      </c>
+      <c r="AU192" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AV192" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="AW192" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="AX192" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="193" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A193" s="7">
+        <v>45887.755224606481</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C193" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D193" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E193" s="8" t="s">
+        <v>630</v>
+      </c>
+      <c r="F193" s="8">
+        <v>4</v>
+      </c>
+      <c r="G193" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H193" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I193" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J193" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K193" s="8">
+        <v>4</v>
+      </c>
+      <c r="L193" s="8">
+        <v>4</v>
+      </c>
+      <c r="M193" s="8">
+        <v>4</v>
+      </c>
+      <c r="N193" s="8">
+        <v>4</v>
+      </c>
+      <c r="O193" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P193" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q193" s="8">
+        <v>4</v>
+      </c>
+      <c r="R193" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="S193" s="8">
+        <v>4</v>
+      </c>
+      <c r="T193" s="8">
+        <v>4</v>
+      </c>
+      <c r="U193" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="V193" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="W193" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="X193" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y193" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z193" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA193" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB193" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC193" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD193" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE193" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF193" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG193" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="AH193" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="AI193" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="AJ193" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="AK193" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM193" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN193" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AO193" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ193" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR193" s="8" t="s">
+        <v>632</v>
+      </c>
+      <c r="AS193" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT193" s="8" t="s">
+        <v>1057</v>
+      </c>
+      <c r="AU193" s="8" t="s">
+        <v>1058</v>
+      </c>
+      <c r="AV193" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW193" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX193" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="194" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A194" s="4">
+        <v>45887.801539479166</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C194" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D194" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E194" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F194" s="5">
+        <v>5</v>
+      </c>
+      <c r="G194" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H194" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="I194" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J194" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K194" s="5">
+        <v>4</v>
+      </c>
+      <c r="L194" s="5">
+        <v>4</v>
+      </c>
+      <c r="M194" s="5">
+        <v>4</v>
+      </c>
+      <c r="N194" s="5">
+        <v>5</v>
+      </c>
+      <c r="O194" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P194" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q194" s="5">
+        <v>5</v>
+      </c>
+      <c r="R194" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="S194" s="5">
+        <v>4</v>
+      </c>
+      <c r="T194" s="5">
+        <v>4</v>
+      </c>
+      <c r="U194" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V194" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W194" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="X194" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y194" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z194" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA194" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB194" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC194" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD194" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE194" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF194" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG194" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="AH194" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI194" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="AJ194" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="AK194" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM194" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN194" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ194" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR194" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="AS194" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT194" s="5" t="s">
+        <v>1059</v>
+      </c>
+      <c r="AU194" s="5" t="s">
+        <v>1060</v>
+      </c>
+      <c r="AV194" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="AW194" s="5" t="s">
+        <v>1061</v>
+      </c>
+      <c r="AX194" s="5" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="195" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A195" s="7">
+        <v>45888.153305196756</v>
+      </c>
+      <c r="B195" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C195" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D195" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E195" s="8" t="s">
+        <v>630</v>
+      </c>
+      <c r="F195" s="8">
+        <v>5</v>
+      </c>
+      <c r="G195" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H195" s="8" t="s">
+        <v>1062</v>
+      </c>
+      <c r="I195" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J195" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K195" s="8">
+        <v>5</v>
+      </c>
+      <c r="L195" s="8">
+        <v>5</v>
+      </c>
+      <c r="M195" s="8">
+        <v>4</v>
+      </c>
+      <c r="N195" s="8">
+        <v>5</v>
+      </c>
+      <c r="O195" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P195" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q195" s="8">
+        <v>5</v>
+      </c>
+      <c r="R195" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="S195" s="8">
+        <v>5</v>
+      </c>
+      <c r="T195" s="8">
+        <v>5</v>
+      </c>
+      <c r="U195" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="V195" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="W195" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="X195" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y195" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z195" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA195" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB195" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC195" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD195" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE195" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF195" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG195" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="AH195" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI195" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="AJ195" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="AK195" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM195" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN195" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ195" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR195" s="8" t="s">
+        <v>657</v>
+      </c>
+      <c r="AS195" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AT195" s="8" t="s">
+        <v>1063</v>
+      </c>
+      <c r="AU195" s="8" t="s">
+        <v>1064</v>
+      </c>
+      <c r="AV195" s="8" t="s">
+        <v>1065</v>
+      </c>
+      <c r="AW195" s="8" t="s">
+        <v>672</v>
+      </c>
+      <c r="AX195" s="8" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="196" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A196" s="4">
+        <v>45888.421498055555</v>
+      </c>
+      <c r="B196" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C196" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D196" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E196" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="F196" s="5">
+        <v>2</v>
+      </c>
+      <c r="G196" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I196" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J196" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K196" s="5">
+        <v>3</v>
+      </c>
+      <c r="L196" s="5">
+        <v>5</v>
+      </c>
+      <c r="M196" s="5">
+        <v>4</v>
+      </c>
+      <c r="N196" s="5">
+        <v>4</v>
+      </c>
+      <c r="O196" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P196" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q196" s="5">
+        <v>4</v>
+      </c>
+      <c r="R196" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="S196" s="5">
+        <v>4</v>
+      </c>
+      <c r="T196" s="5">
+        <v>3</v>
+      </c>
+      <c r="U196" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V196" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W196" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="X196" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y196" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z196" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA196" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB196" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC196" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD196" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE196" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF196" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="AG196" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH196" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI196" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ196" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="AK196" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM196" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN196" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ196" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR196" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="AS196" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT196" s="5" t="s">
+        <v>1067</v>
+      </c>
+      <c r="AU196" s="5" t="s">
+        <v>1068</v>
+      </c>
+      <c r="AV196" s="5" t="s">
+        <v>1069</v>
+      </c>
+      <c r="AW196" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="AX196" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="197" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A197" s="7">
+        <v>45888.445674108792</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C197" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D197" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E197" s="8" t="s">
+        <v>630</v>
+      </c>
+      <c r="F197" s="8">
+        <v>4</v>
+      </c>
+      <c r="G197" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I197" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J197" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K197" s="8">
+        <v>4</v>
+      </c>
+      <c r="L197" s="8">
+        <v>4</v>
+      </c>
+      <c r="M197" s="8">
+        <v>3</v>
+      </c>
+      <c r="O197" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="P197" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q197" s="8">
+        <v>3</v>
+      </c>
+      <c r="R197" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="S197" s="8">
+        <v>4</v>
+      </c>
+      <c r="T197" s="8">
+        <v>3</v>
+      </c>
+      <c r="U197" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="V197" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="W197" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="X197" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y197" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z197" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="AA197" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB197" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC197" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD197" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE197" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF197" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG197" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="AH197" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI197" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ197" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="AK197" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM197" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN197" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="AQ197" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR197" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="AS197" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT197" s="8" t="s">
+        <v>1070</v>
+      </c>
+      <c r="AU197" s="8" t="s">
+        <v>1071</v>
+      </c>
+      <c r="AV197" s="8" t="s">
+        <v>1072</v>
+      </c>
+      <c r="AW197" s="8" t="s">
+        <v>1073</v>
+      </c>
+      <c r="AX197" s="8" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="198" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A198" s="4">
+        <v>45888.448251770838</v>
+      </c>
+      <c r="B198" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C198" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D198" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E198" s="5" t="s">
+        <v>932</v>
+      </c>
+      <c r="F198" s="5">
+        <v>5</v>
+      </c>
+      <c r="G198" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H198" s="5" t="s">
+        <v>1074</v>
+      </c>
+      <c r="I198" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J198" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K198" s="5">
+        <v>5</v>
+      </c>
+      <c r="L198" s="5">
+        <v>5</v>
+      </c>
+      <c r="M198" s="5">
+        <v>5</v>
+      </c>
+      <c r="N198" s="5">
+        <v>5</v>
+      </c>
+      <c r="O198" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P198" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q198" s="5">
+        <v>5</v>
+      </c>
+      <c r="R198" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="S198" s="5">
+        <v>5</v>
+      </c>
+      <c r="T198" s="5">
+        <v>5</v>
+      </c>
+      <c r="U198" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V198" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W198" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="X198" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y198" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z198" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA198" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB198" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC198" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD198" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE198" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF198" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG198" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH198" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI198" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="AJ198" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="AK198" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM198" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN198" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="AQ198" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR198" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="AS198" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="AT198" s="5" t="s">
+        <v>1075</v>
+      </c>
+      <c r="AU198" s="5" t="s">
+        <v>1076</v>
+      </c>
+      <c r="AV198" s="5" t="s">
+        <v>1077</v>
+      </c>
+      <c r="AW198" s="5" t="s">
+        <v>1078</v>
+      </c>
+      <c r="AX198" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="199" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A199" s="7">
+        <v>45888.448737013889</v>
+      </c>
+      <c r="B199" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C199" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D199" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E199" s="8" t="s">
+        <v>932</v>
+      </c>
+      <c r="F199" s="8">
+        <v>4</v>
+      </c>
+      <c r="G199" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H199" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="I199" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J199" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K199" s="8">
+        <v>4</v>
+      </c>
+      <c r="L199" s="8">
+        <v>4</v>
+      </c>
+      <c r="M199" s="8">
+        <v>4</v>
+      </c>
+      <c r="N199" s="8">
+        <v>4</v>
+      </c>
+      <c r="O199" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P199" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q199" s="8">
+        <v>4</v>
+      </c>
+      <c r="R199" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="S199" s="8">
+        <v>4</v>
+      </c>
+      <c r="T199" s="8">
+        <v>4</v>
+      </c>
+      <c r="U199" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="V199" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="W199" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="X199" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y199" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z199" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA199" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB199" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC199" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD199" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE199" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF199" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG199" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH199" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI199" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ199" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK199" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM199" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN199" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AO199" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ199" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR199" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="AS199" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT199" s="8" t="s">
+        <v>1079</v>
+      </c>
+      <c r="AU199" s="8" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AV199" s="8" t="s">
+        <v>1081</v>
+      </c>
+      <c r="AW199" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="AX199" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="200" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A200" s="4">
+        <v>45888.456692361113</v>
+      </c>
+      <c r="B200" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C200" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D200" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E200" s="5" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F200" s="5">
+        <v>4</v>
+      </c>
+      <c r="G200" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I200" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J200" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K200" s="5">
+        <v>4</v>
+      </c>
+      <c r="L200" s="5">
+        <v>4</v>
+      </c>
+      <c r="M200" s="5">
+        <v>5</v>
+      </c>
+      <c r="N200" s="5">
+        <v>5</v>
+      </c>
+      <c r="O200" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P200" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q200" s="5">
+        <v>4</v>
+      </c>
+      <c r="R200" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="S200" s="5">
+        <v>4</v>
+      </c>
+      <c r="T200" s="5">
+        <v>5</v>
+      </c>
+      <c r="U200" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V200" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W200" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="X200" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y200" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z200" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA200" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB200" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC200" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD200" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE200" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF200" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG200" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH200" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI200" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="AJ200" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK200" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM200" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN200" s="5" t="s">
+        <v>1083</v>
+      </c>
+      <c r="AQ200" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR200" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="AS200" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT200" s="5" t="s">
+        <v>1084</v>
+      </c>
+      <c r="AU200" s="5" t="s">
+        <v>1085</v>
+      </c>
+      <c r="AV200" s="5" t="s">
+        <v>1086</v>
+      </c>
+      <c r="AW200" s="5" t="s">
+        <v>1087</v>
+      </c>
+      <c r="AX200" s="5" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="201" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A201" s="7">
+        <v>45888.505566203705</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C201" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="D201" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I201" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP201" s="8" t="s">
+        <v>1088</v>
+      </c>
+      <c r="AQ201" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR201" s="8" t="s">
+        <v>1089</v>
+      </c>
+      <c r="AS201" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AT201" s="8" t="s">
+        <v>1090</v>
+      </c>
+      <c r="AU201" s="8" t="s">
+        <v>1091</v>
+      </c>
+      <c r="AV201" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW201" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="AX201" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="202" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A202" s="4">
+        <v>45888.509473819446</v>
+      </c>
+      <c r="B202" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C202" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="D202" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E202" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="F202" s="5">
+        <v>5</v>
+      </c>
+      <c r="G202" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H202" s="5" t="s">
+        <v>1092</v>
+      </c>
+      <c r="I202" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J202" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K202" s="5">
+        <v>4</v>
+      </c>
+      <c r="L202" s="5">
+        <v>5</v>
+      </c>
+      <c r="M202" s="5">
+        <v>5</v>
+      </c>
+      <c r="N202" s="5">
+        <v>5</v>
+      </c>
+      <c r="O202" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P202" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q202" s="5">
+        <v>4</v>
+      </c>
+      <c r="R202" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="S202" s="5">
+        <v>5</v>
+      </c>
+      <c r="T202" s="5">
+        <v>5</v>
+      </c>
+      <c r="U202" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V202" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W202" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="X202" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y202" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z202" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA202" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB202" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC202" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD202" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE202" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF202" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG202" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH202" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI202" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="AJ202" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK202" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM202" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN202" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="AQ202" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR202" s="5" t="s">
+        <v>955</v>
+      </c>
+      <c r="AS202" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT202" s="5" t="s">
+        <v>1093</v>
+      </c>
+      <c r="AU202" s="5" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AV202" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="AW202" s="5" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AX202" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="203" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A203" s="7">
+        <v>45888.515778356479</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C203" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="D203" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E203" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="F203" s="8">
+        <v>4</v>
+      </c>
+      <c r="G203" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I203" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J203" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K203" s="8">
+        <v>3</v>
+      </c>
+      <c r="L203" s="8">
+        <v>3</v>
+      </c>
+      <c r="M203" s="8">
+        <v>3</v>
+      </c>
+      <c r="N203" s="8">
+        <v>3</v>
+      </c>
+      <c r="O203" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="P203" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q203" s="8">
+        <v>3</v>
+      </c>
+      <c r="R203" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="S203" s="8">
+        <v>2</v>
+      </c>
+      <c r="T203" s="8">
+        <v>4</v>
+      </c>
+      <c r="U203" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="V203" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="W203" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="X203" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y203" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z203" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA203" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB203" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC203" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD203" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE203" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF203" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG203" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH203" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI203" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="AJ203" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="AK203" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL203" s="8" t="s">
+        <v>1096</v>
+      </c>
+      <c r="AM203" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN203" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AO203" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ203" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR203" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="AS203" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT203" s="8" t="s">
+        <v>1097</v>
+      </c>
+      <c r="AU203" s="8" t="s">
+        <v>1098</v>
+      </c>
+      <c r="AV203" s="8" t="s">
+        <v>1099</v>
+      </c>
+      <c r="AW203" s="8" t="s">
+        <v>1100</v>
+      </c>
+      <c r="AX203" s="8" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="204" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A204" s="4">
+        <v>45888.604604259264</v>
+      </c>
+      <c r="B204" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C204" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="D204" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E204" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="F204" s="5">
+        <v>5</v>
+      </c>
+      <c r="G204" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H204" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I204" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ204" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR204" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="AS204" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT204" s="5" t="s">
+        <v>1102</v>
+      </c>
+      <c r="AU204" s="5" t="s">
+        <v>1103</v>
+      </c>
+      <c r="AV204" s="5" t="s">
+        <v>1104</v>
+      </c>
+      <c r="AW204" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="AX204" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="205" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A205" s="7">
+        <v>45888.678354548611</v>
+      </c>
+      <c r="B205" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C205" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D205" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E205" s="8" t="s">
+        <v>853</v>
+      </c>
+      <c r="F205" s="8">
+        <v>5</v>
+      </c>
+      <c r="G205" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H205" s="8" t="s">
+        <v>854</v>
+      </c>
+      <c r="I205" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP205" s="8" t="s">
+        <v>1105</v>
+      </c>
+      <c r="AQ205" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR205" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AS205" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT205" s="8" t="s">
+        <v>1106</v>
+      </c>
+      <c r="AU205" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AV205" s="8" t="s">
+        <v>1107</v>
+      </c>
+      <c r="AW205" s="8" t="s">
+        <v>1108</v>
+      </c>
+      <c r="AX205" s="8" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="206" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A206" s="4">
+        <v>45888.681487847221</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C206" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D206" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E206" s="5" t="s">
+        <v>853</v>
+      </c>
+      <c r="F206" s="5">
+        <v>5</v>
+      </c>
+      <c r="G206" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H206" s="5" t="s">
+        <v>1110</v>
+      </c>
+      <c r="I206" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J206" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K206" s="5">
+        <v>5</v>
+      </c>
+      <c r="L206" s="5">
+        <v>5</v>
+      </c>
+      <c r="M206" s="5">
+        <v>5</v>
+      </c>
+      <c r="N206" s="5">
+        <v>5</v>
+      </c>
+      <c r="O206" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P206" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q206" s="5">
+        <v>5</v>
+      </c>
+      <c r="R206" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="S206" s="5">
+        <v>5</v>
+      </c>
+      <c r="T206" s="5">
+        <v>5</v>
+      </c>
+      <c r="U206" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V206" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W206" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="X206" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="Y206" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z206" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA206" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB206" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC206" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD206" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE206" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF206" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG206" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="AH206" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AI206" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ206" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK206" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="AM206" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN206" s="5" t="s">
+        <v>1111</v>
+      </c>
+      <c r="AQ206" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR206" s="5" t="s">
+        <v>1089</v>
+      </c>
+      <c r="AS206" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT206" s="5" t="s">
+        <v>1112</v>
+      </c>
+      <c r="AU206" s="5" t="s">
+        <v>1113</v>
+      </c>
+      <c r="AV206" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="AW206" s="5" t="s">
+        <v>1114</v>
+      </c>
+      <c r="AX206" s="5" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="207" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+      <c r="A207" s="10">
+        <v>45888.699615069447</v>
+      </c>
+      <c r="B207" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C207" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D207" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E207" s="11" t="s">
+        <v>1115</v>
+      </c>
+      <c r="F207" s="11">
+        <v>5</v>
+      </c>
+      <c r="G207" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H207" s="11" t="s">
+        <v>1116</v>
+      </c>
+      <c r="I207" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J207" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="K207" s="11">
+        <v>5</v>
+      </c>
+      <c r="L207" s="11">
+        <v>5</v>
+      </c>
+      <c r="M207" s="11">
+        <v>4</v>
+      </c>
+      <c r="N207" s="11">
+        <v>5</v>
+      </c>
+      <c r="O207" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="P207" s="11">
+        <v>5</v>
+      </c>
+      <c r="Q207" s="11">
+        <v>5</v>
+      </c>
+      <c r="R207" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="S207" s="11">
+        <v>5</v>
+      </c>
+      <c r="T207" s="11">
+        <v>4</v>
+      </c>
+      <c r="U207" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="V207" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="W207" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="X207" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y207" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z207" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA207" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB207" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC207" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD207" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE207" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF207" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG207" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH207" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="AI207" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="AJ207" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="AK207" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL207" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM207" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN207" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="AO207" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ207" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR207" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="AS207" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT207" s="11" t="s">
+        <v>1117</v>
+      </c>
+      <c r="AU207" s="11" t="s">
+        <v>1118</v>
+      </c>
+      <c r="AV207" s="11" t="s">
+        <v>1119</v>
+      </c>
+      <c r="AW207" s="11" t="s">
+        <v>438</v>
+      </c>
+      <c r="AX207" s="11" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -27948,7 +30598,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="D1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -27957,7 +30607,311 @@
     <col min="1" max="1" width="38" customWidth="1"/>
     <col min="2" max="2" width="27.83203125" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D1" s="12" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="2" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D2" s="12">
+        <v>19</v>
+      </c>
+      <c r="E2" s="13">
+        <f t="shared" ref="E2:E33" si="0">C2/D2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D3" s="12">
+        <v>9</v>
+      </c>
+      <c r="E3" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D4" s="12">
+        <f>SUM(D2:D3)</f>
+        <v>28</v>
+      </c>
+      <c r="E4" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D5" s="12">
+        <v>11</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D6" s="12">
+        <v>12</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D7" s="12">
+        <v>6</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D8" s="12">
+        <v>10</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D9" s="12">
+        <v>13</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D10" s="12">
+        <v>7</v>
+      </c>
+      <c r="E10" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D11" s="12">
+        <v>11</v>
+      </c>
+      <c r="E11" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D12" s="12">
+        <v>12</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D13" s="12">
+        <v>11</v>
+      </c>
+      <c r="E13" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D14" s="12">
+        <f>SUM(D5:D13)</f>
+        <v>93</v>
+      </c>
+      <c r="E14" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D15" s="12">
+        <v>7</v>
+      </c>
+      <c r="E15" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D16" s="12">
+        <v>7</v>
+      </c>
+      <c r="E16" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D17" s="12">
+        <f>SUM(D15:D16)</f>
+        <v>14</v>
+      </c>
+      <c r="E17" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D18" s="12">
+        <v>6</v>
+      </c>
+      <c r="E18" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D19" s="12">
+        <v>9</v>
+      </c>
+      <c r="E19" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D20" s="12">
+        <v>8</v>
+      </c>
+      <c r="E20" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D21" s="12">
+        <v>10</v>
+      </c>
+      <c r="E21" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D22" s="12">
+        <v>9</v>
+      </c>
+      <c r="E22" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D23" s="12">
+        <v>9</v>
+      </c>
+      <c r="E23" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D24" s="12">
+        <v>14</v>
+      </c>
+      <c r="E24" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D25" s="12">
+        <f>SUM(D18:D24)</f>
+        <v>65</v>
+      </c>
+      <c r="E25" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D26" s="12">
+        <v>3</v>
+      </c>
+      <c r="E26" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D27" s="12">
+        <v>8</v>
+      </c>
+      <c r="E27" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D28" s="12">
+        <v>7</v>
+      </c>
+      <c r="E28" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D29" s="12">
+        <v>10</v>
+      </c>
+      <c r="E29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D30" s="12">
+        <v>13</v>
+      </c>
+      <c r="E30" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D31" s="12">
+        <v>9</v>
+      </c>
+      <c r="E31" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D32" s="12">
+        <f>SUM(D26:D31)</f>
+        <v>50</v>
+      </c>
+      <c r="E32" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D33" s="12">
+        <f>D4+D14+D17+D25+D32</f>
+        <v>250</v>
+      </c>
+      <c r="E33" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>